<commit_message>
Finished some of tasks from Excel file and added a few new ones
</commit_message>
<xml_diff>
--- a/ShelfItService/taski-WebAPI.xlsx
+++ b/ShelfItService/taski-WebAPI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Radek\Desktop\Inżynierka\ShelfItWebAPI\ShelfItService\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B39BE7-2E3D-4A74-851C-64CDEDF2950E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72A83A5-5B62-4B5B-964C-1578AD86C96E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2FF065FE-796E-4DF0-9A4C-3C3C7D12D268}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="44">
   <si>
     <t>Zadanie</t>
   </si>
@@ -96,15 +96,9 @@
     <t>Należy dodać metody, które pozwolą na zapraszanie użytkowników po adresie email do dołączenia do bazy użytkowników aplikacji</t>
   </si>
   <si>
-    <t>W trakcie</t>
-  </si>
-  <si>
     <t>Taski - WebAPI</t>
   </si>
   <si>
-    <t>tabela z adresami email, treść maila</t>
-  </si>
-  <si>
     <t>Tabela z emailami</t>
   </si>
   <si>
@@ -117,22 +111,58 @@
     <t>W każdym kontrolerze należy zamienić dziedziczenie z klasy Controller na dziedziczenie z klasy DefaultController i zamienić bezpośrednie wywołania odpowiedzi BadRequest na wywołania metod z DefaultController</t>
   </si>
   <si>
-    <t>pozostałe kontrolery: LoginController, MusicController</t>
-  </si>
-  <si>
     <t>Usuwanie zmienionego hasła</t>
   </si>
   <si>
     <t>Dodanie metody która umożliwi użytkownikowi reset hasła, w sytuacji gdyby to nie użytkownik zmienił hasło</t>
   </si>
   <si>
-    <t>metoda stworzona, należy dodać logikę</t>
-  </si>
-  <si>
     <t>Modyfikacja bazy danych</t>
   </si>
   <si>
     <t>Dodanie pól do użytkownika: reset hasła i deaktywacja konta</t>
+  </si>
+  <si>
+    <t>Zakończone</t>
+  </si>
+  <si>
+    <t>Przeniesione</t>
+  </si>
+  <si>
+    <t>Przeniesione do zadania 11</t>
+  </si>
+  <si>
+    <t>Uzupełnienie tabeli z emailami</t>
+  </si>
+  <si>
+    <t>Należy przenieść wszystkie istniejące oraz dodać te brakujące emaile, które obecnie znajdują się w statycznym repozytorium, do tabeli na bazie danych.</t>
+  </si>
+  <si>
+    <t>Wyczyszczenie repozytoriów</t>
+  </si>
+  <si>
+    <t>W momencie kiedy nie będą już potrzebne, należy wyczyścić statyczne repozytoria oraz wszystkie odniesienia do nich w kodzie</t>
+  </si>
+  <si>
+    <t>Usuwanie filmów</t>
+  </si>
+  <si>
+    <t>Dodać metodę do usuwania filmów z bazy</t>
+  </si>
+  <si>
+    <t>Przeniesione do zadania 14</t>
+  </si>
+  <si>
+    <t>Refactoring Music Controllera</t>
+  </si>
+  <si>
+    <t>Należy usunąć wszystkie nieużywane i przestarzałe metody z kontrollera</t>
+  </si>
+  <si>
+    <t>Usuwanie muzyki</t>
+  </si>
+  <si>
+    <t>Dodać metodę do usuwania muzyki z bazy</t>
   </si>
 </sst>
 </file>
@@ -500,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1B454C2-521F-474E-BDB9-9AAA8A3EFC56}">
-  <dimension ref="C1:G13"/>
+  <dimension ref="C1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -517,7 +547,7 @@
   <sheetData>
     <row r="1" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C1" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
@@ -644,10 +674,10 @@
         <v>20</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="3:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -655,16 +685,16 @@
         <v>7</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="3:7" ht="86.4" x14ac:dyDescent="0.3">
@@ -672,16 +702,16 @@
         <v>8</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="3:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -689,34 +719,136 @@
         <v>9</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>31</v>
-      </c>
+      <c r="G12" s="2"/>
     </row>
     <row r="13" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C13" s="1">
         <v>10</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="3:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="C14" s="1">
+        <v>11</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G13" s="2" t="s">
+      <c r="E14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>7</v>
       </c>
+    </row>
+    <row r="15" spans="3:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C15" s="1">
+        <v>12</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C16" s="2">
+        <v>13</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C17" s="2">
+        <v>14</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C18" s="2">
+        <v>15</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
deleting music and movies, added emails
</commit_message>
<xml_diff>
--- a/ShelfItService/taski-WebAPI.xlsx
+++ b/ShelfItService/taski-WebAPI.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Radek\Desktop\Inżynierka\ShelfItWebAPI\ShelfItService\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E0C574-031D-48F0-8719-3347E68355FE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2FF065FE-796E-4DF0-9A4C-3C3C7D12D268}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -18,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Arkusz1!$F$1:$F$21</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -177,7 +171,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -285,7 +279,7 @@
     </a:clrScheme>
     <a:fontScheme name="Pakiet Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -337,7 +331,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -531,19 +525,19 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1B454C2-521F-474E-BDB9-9AAA8A3EFC56}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
   <dimension ref="C1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F3" sqref="F1:F1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -801,7 +795,7 @@
         <v>34</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>45</v>
@@ -841,7 +835,7 @@
         <v>38</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>45</v>
@@ -881,7 +875,7 @@
         <v>43</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>45</v>
@@ -915,7 +909,7 @@
       <c r="H21" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="F1:F21" xr:uid="{4DE2B74A-5E00-4919-B69D-CE4823E65D0D}">
+  <autoFilter ref="F1:F21">
     <filterColumn colId="0">
       <filters>
         <filter val="Nie rozpoczęte"/>

</xml_diff>